<commit_message>
fix bug in dot charts
</commit_message>
<xml_diff>
--- a/data-viz/inputs/region_labels.xlsx
+++ b/data-viz/inputs/region_labels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wjproject.sharepoint.com/research/Programmatic/EU Subnational/EU-S Data/reports/eu-thematic-reports/data-viz/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="413" documentId="8_{6626208B-8827-4CBE-9772-3AA277DEA2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D53809CE-80C5-46C4-9E36-28421E7F2FB9}"/>
+  <xr:revisionPtr revIDLastSave="415" documentId="8_{6626208B-8827-4CBE-9772-3AA277DEA2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0411938-89AF-814A-A000-CF3F78F2834A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{DD3ABE5B-D581-4517-9DBD-9419A819EBBB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{DD3ABE5B-D581-4517-9DBD-9419A819EBBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1902,6 +1902,7 @@
     <font>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -2019,10 +2020,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2322,24 +2319,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B15BD7-531B-4529-B0B4-38B6E533B250}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:K122"/>
+  <dimension ref="A1:K111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I122" sqref="I29:I122"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.453125" customWidth="1"/>
-    <col min="4" max="4" width="48.36328125" customWidth="1"/>
-    <col min="5" max="5" width="39.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="48.33203125" customWidth="1"/>
+    <col min="5" max="5" width="39.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" style="15"/>
+    <col min="9" max="9" width="11.5" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>324</v>
       </c>
@@ -2374,7 +2370,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>222</v>
       </c>
@@ -2410,7 +2406,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>222</v>
       </c>
@@ -2446,7 +2442,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>222</v>
       </c>
@@ -2482,7 +2478,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2518,7 +2514,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -2554,7 +2550,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -2590,7 +2586,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -2626,7 +2622,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2662,7 +2658,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -2698,7 +2694,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>155</v>
       </c>
@@ -2734,7 +2730,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>155</v>
       </c>
@@ -2770,7 +2766,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>155</v>
       </c>
@@ -2806,7 +2802,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>182</v>
       </c>
@@ -2842,7 +2838,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
         <v>17</v>
       </c>
@@ -2878,7 +2874,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
         <v>17</v>
       </c>
@@ -2914,7 +2910,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
         <v>17</v>
       </c>
@@ -2950,7 +2946,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
         <v>17</v>
       </c>
@@ -2986,7 +2982,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -3022,7 +3018,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -3058,7 +3054,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -3094,7 +3090,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -3130,7 +3126,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -3166,7 +3162,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -3202,7 +3198,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>300</v>
       </c>
@@ -3238,7 +3234,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>300</v>
       </c>
@@ -3274,7 +3270,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
         <v>300</v>
       </c>
@@ -3310,7 +3306,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>300</v>
       </c>
@@ -3346,7 +3342,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>121</v>
       </c>
@@ -3382,7 +3378,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>121</v>
       </c>
@@ -3418,7 +3414,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>121</v>
       </c>
@@ -3454,7 +3450,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>121</v>
       </c>
@@ -3490,7 +3486,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>121</v>
       </c>
@@ -3526,7 +3522,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>121</v>
       </c>
@@ -3562,7 +3558,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>121</v>
       </c>
@@ -3598,7 +3594,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>121</v>
       </c>
@@ -3634,7 +3630,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>121</v>
       </c>
@@ -3670,7 +3666,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>121</v>
       </c>
@@ -3706,7 +3702,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>121</v>
       </c>
@@ -3742,7 +3738,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>121</v>
       </c>
@@ -3778,7 +3774,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>121</v>
       </c>
@@ -3814,7 +3810,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>38</v>
       </c>
@@ -3850,7 +3846,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>38</v>
       </c>
@@ -3886,7 +3882,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -3922,7 +3918,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>38</v>
       </c>
@@ -3958,7 +3954,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>38</v>
       </c>
@@ -3994,7 +3990,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>38</v>
       </c>
@@ -4030,7 +4026,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>38</v>
       </c>
@@ -4066,7 +4062,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>38</v>
       </c>
@@ -4102,7 +4098,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>38</v>
       </c>
@@ -4138,7 +4134,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>38</v>
       </c>
@@ -4174,7 +4170,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>38</v>
       </c>
@@ -4210,7 +4206,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>38</v>
       </c>
@@ -4246,7 +4242,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>38</v>
       </c>
@@ -4282,7 +4278,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>38</v>
       </c>
@@ -4318,7 +4314,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>38</v>
       </c>
@@ -4354,7 +4350,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>38</v>
       </c>
@@ -4390,7 +4386,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>89</v>
       </c>
@@ -4426,7 +4422,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>89</v>
       </c>
@@ -4462,7 +4458,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>89</v>
       </c>
@@ -4498,7 +4494,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>89</v>
       </c>
@@ -4534,7 +4530,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>197</v>
       </c>
@@ -4570,7 +4566,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>197</v>
       </c>
@@ -4606,7 +4602,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>197</v>
       </c>
@@ -4642,7 +4638,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>82</v>
       </c>
@@ -4678,7 +4674,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>82</v>
       </c>
@@ -4714,7 +4710,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>82</v>
       </c>
@@ -4750,7 +4746,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>169</v>
       </c>
@@ -4786,7 +4782,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>169</v>
       </c>
@@ -4822,7 +4818,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>169</v>
       </c>
@@ -4858,7 +4854,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>169</v>
       </c>
@@ -4894,7 +4890,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>169</v>
       </c>
@@ -4930,7 +4926,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>185</v>
       </c>
@@ -4966,7 +4962,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>188</v>
       </c>
@@ -5002,7 +4998,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>188</v>
       </c>
@@ -5038,7 +5034,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>195</v>
       </c>
@@ -5074,7 +5070,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>207</v>
       </c>
@@ -5110,7 +5106,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>209</v>
       </c>
@@ -5146,7 +5142,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>209</v>
       </c>
@@ -5182,7 +5178,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>209</v>
       </c>
@@ -5218,7 +5214,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>209</v>
       </c>
@@ -5254,7 +5250,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>232</v>
       </c>
@@ -5290,7 +5286,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>232</v>
       </c>
@@ -5326,7 +5322,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>232</v>
       </c>
@@ -5362,7 +5358,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>232</v>
       </c>
@@ -5398,7 +5394,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>232</v>
       </c>
@@ -5434,7 +5430,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>232</v>
       </c>
@@ -5470,7 +5466,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>232</v>
       </c>
@@ -5506,7 +5502,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>254</v>
       </c>
@@ -5542,7 +5538,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>254</v>
       </c>
@@ -5578,7 +5574,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>254</v>
       </c>
@@ -5614,7 +5610,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>266</v>
       </c>
@@ -5650,7 +5646,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>266</v>
       </c>
@@ -5686,7 +5682,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>266</v>
       </c>
@@ -5722,7 +5718,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>266</v>
       </c>
@@ -5758,7 +5754,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>286</v>
       </c>
@@ -5794,7 +5790,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>286</v>
       </c>
@@ -5830,7 +5826,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>286</v>
       </c>
@@ -5866,7 +5862,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>286</v>
       </c>
@@ -5902,7 +5898,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>279</v>
       </c>
@@ -5938,7 +5934,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>279</v>
       </c>
@@ -5974,7 +5970,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>102</v>
       </c>
@@ -6010,7 +6006,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -6046,7 +6042,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>102</v>
       </c>
@@ -6082,7 +6078,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>102</v>
       </c>
@@ -6118,7 +6114,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>102</v>
       </c>
@@ -6154,7 +6150,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>102</v>
       </c>
@@ -6190,7 +6186,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>102</v>
       </c>
@@ -6226,7 +6222,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>309</v>
       </c>
@@ -6262,7 +6258,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>309</v>
       </c>
@@ -6298,7 +6294,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>309</v>
       </c>
@@ -6334,30 +6330,8 @@
         <v>589</v>
       </c>
     </row>
-    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="113" spans="9:9" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="114" spans="9:9" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="115" spans="9:9" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="116" spans="9:9" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="117" spans="9:9" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="118" spans="9:9" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="119" spans="9:9" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="120" spans="9:9" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="121" spans="9:9" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="122" spans="9:9" x14ac:dyDescent="0.35">
-      <c r="I122" s="15">
-        <f>SUBTOTAL(9,I29:I121)</f>
-        <v>0.96703949132219935</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:K121" xr:uid="{A7B15BD7-531B-4529-B0B4-38B6E533B250}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="France"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K121" xr:uid="{A7B15BD7-531B-4529-B0B4-38B6E533B250}"/>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6376,6 +6350,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BF094976B1C6245BAB5BCECAC284645" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3620e9c0d1a16779aea146adda0186f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="69276225-f05c-44c5-92dc-c999460a4149" xmlns:ns3="46f3a809-46a3-44ee-a0f1-42a271529c86" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f2afd3ea0446edf26a13b3c7fc9e6232" ns2:_="" ns3:_="">
     <xsd:import namespace="69276225-f05c-44c5-92dc-c999460a4149"/>
@@ -6624,33 +6607,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51C746D7-CF54-4E7D-92A4-AB36B233844F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
+    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A3263D7-CA43-48BC-8F28-1FA6213EFCDC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED2CE6EF-790B-4B69-B141-5B1187A2316D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6667,12 +6649,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A3263D7-CA43-48BC-8F28-1FA6213EFCDC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>